<commit_message>
Add destination_plate parameter to README
</commit_message>
<xml_diff>
--- a/Plater/dest_plate_for_data_csv.xlsx
+++ b/Plater/dest_plate_for_data_csv.xlsx
@@ -522,10 +522,26 @@
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>p19_mtagbfp2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>p24_3'ha_haavs1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>p6_nt-igkl sequence</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>p8_p2a</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -557,10 +573,26 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>p19_tet-on-3g</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>p24_3'pb</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>p6_nt-mls</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>p8a_ct-kdel</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -592,10 +624,26 @@
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>p1_5'-itr-pb</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>p25_sv40-ori</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>p6_nt-myristoylation signal</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>p8b_ires2</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -627,10 +675,26 @@
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>p1_5'ha-haavs1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>p2_insulatorfb</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>p6_nt-palm sequence</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>p9_a-tubulin</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
@@ -662,10 +726,26 @@
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>p20_ct-minute-nes</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>p3_cagp</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>p6_nt-sv40_nls</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>p9_bsdr</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
@@ -697,10 +777,26 @@
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>p20_ct-nes</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>p3_cmvp_tet</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>p7_bxb1</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>p9_dmrc</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
@@ -732,10 +828,26 @@
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>p20_linker3</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>p3_ef1ap</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>p7_l7ae-weiss</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>p9_firefly_luciferase</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -767,10 +879,26 @@
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>p20_p2a</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>p3_tre3gp</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>p7_l7ae</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>p9_mneogreen</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
@@ -802,10 +930,26 @@
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>p21_dmra</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>p4_kt-l7ae -weiss</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>p7_laci</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>p9_mruby2</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
@@ -837,10 +981,26 @@
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>p21_mkate2</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>p4_lac-o</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>p7_mcherry</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>p9_mtagbfp2</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -872,10 +1032,26 @@
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>p21_mneogreen</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>p5_attb-bxb1</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>p7_mkate2</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>p9_neor</t>
+        </is>
+      </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
@@ -903,10 +1079,26 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>p21_mruby2</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>p5_attp-bxb1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>p7_mneogreen</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>p9_puror</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -934,9 +1126,21 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>p21_mtagbfp2</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>p5_k1-k1</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>p7_mruby2</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
@@ -965,9 +1169,21 @@
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>p21_puror</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>p5_kt-weiss</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>p7_mtagbfp2</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
@@ -996,9 +1212,21 @@
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>p22_pgkpolya</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>p6_atg_boxc</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>p8_linker1</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
@@ -1017,7 +1245,11 @@
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>WATER</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1027,9 +1259,21 @@
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>p23_insulatorfb</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>p6_kozak-atg</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>p8_linker2</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -1048,7 +1292,11 @@
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>BUFFER</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1156,16 +1404,16 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1235,16 +1483,16 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -1314,16 +1562,16 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -1393,16 +1641,16 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -1472,16 +1720,16 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -1551,16 +1799,16 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1630,16 +1878,16 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1709,16 +1957,16 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1788,16 +2036,16 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1867,16 +2115,16 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1946,16 +2194,16 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -2025,16 +2273,16 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -2104,13 +2352,13 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -2183,13 +2431,13 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -2262,13 +2510,13 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -2325,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="Y16" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17">
@@ -2341,13 +2589,13 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -2404,7 +2652,7 @@
         <v>0</v>
       </c>
       <c r="Y17" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2513,16 +2761,16 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>68.7</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>68.7</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -2592,16 +2840,16 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>98.3</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>52.8</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>86.00000000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>98.3</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -2671,16 +2919,16 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>68.3</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>46.4</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>73.7</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>68.3</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -2750,16 +2998,16 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>80.3</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>59.3</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>69.5</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>80.3</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -2829,16 +3077,16 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>111.1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>56.1</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>111.1</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -2908,16 +3156,16 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>76.3</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>106.7</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>63.4</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>76.3</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -2987,16 +3235,16 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>77.3</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>70.3</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>44.6</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>77.3</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -3066,16 +3314,16 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>68.7</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>62.40000000000001</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -3145,16 +3393,16 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>50.1</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>98.3</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>226</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>50.1</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -3224,16 +3472,16 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>68.3</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -3303,16 +3551,16 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>52.8</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>80.3</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>52.8</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>52.8</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -3382,16 +3630,16 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>46.4</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>111.1</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>46.4</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>46.4</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -3461,13 +3709,13 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>59.3</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>76.3</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>59.3</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -3540,13 +3788,13 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>77.3</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -3619,13 +3867,13 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>106.7</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>80.09999999999999</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>106.7</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -3682,7 +3930,7 @@
         <v>0</v>
       </c>
       <c r="Y16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -3698,13 +3946,13 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>70.3</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>50.1</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>70.3</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -3761,7 +4009,7 @@
         <v>0</v>
       </c>
       <c r="Y17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>